<commit_message>
Reformatted the code. Updated README.md file. Added Performance testing code. Added executable .bat and .sh files for the ease of execution.
</commit_message>
<xml_diff>
--- a/Test Suite.xlsx
+++ b/Test Suite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garthbosch/projects/personal/stitchmoney-assessment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF69262-1A99-FB45-BF5D-8CBDB04DD543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF6F195-C60D-4740-B5ED-AC3A9C1E6E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19980" xr2:uid="{E34D0DFE-D57E-C243-964C-D1A7B67EAB68}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19980" activeTab="1" xr2:uid="{E34D0DFE-D57E-C243-964C-D1A7B67EAB68}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -126,22 +126,68 @@
   </si>
   <si>
     <t>API</t>
+  </si>
+  <si>
+    <t>Test Scenario</t>
+  </si>
+  <si>
+    <t>Actual Result</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>Delete all the items from the list via API or GUI.</t>
+  </si>
+  <si>
+    <t>The user can successfully delete a item with done status</t>
+  </si>
+  <si>
+    <t>An error message should appear and the item should not be added.</t>
+  </si>
+  <si>
+    <t>An error message should appear and the user should be blocked.</t>
+  </si>
+  <si>
+    <t>All items can be deleted. The list should not be empty.</t>
+  </si>
+  <si>
+    <t>A user should be able to edit a Todo List item.</t>
+  </si>
+  <si>
+    <t>Duplicated entries can be added to the list.</t>
+  </si>
+  <si>
+    <t>The item with incorrect character length successfully added.</t>
+  </si>
+  <si>
+    <t>Duplicated entry added.</t>
+  </si>
+  <si>
+    <t>Test can have no items in it.</t>
+  </si>
+  <si>
+    <t>There's no option to edit an item form the list.</t>
+  </si>
+  <si>
+    <t>From the front end it does not allow you to edit an item.</t>
+  </si>
+  <si>
+    <t>Items which are in DONE status can be deleted via the API and the GUI.</t>
+  </si>
+  <si>
+    <t>An item with 100 or more can characters can be added to the list.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -155,6 +201,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -164,7 +233,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -187,28 +256,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -216,26 +299,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -561,231 +624,231 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F2AF6D-306D-CC4E-80B9-028969904735}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.1640625" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" s="8" customFormat="1" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="6"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="6"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="6"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -923,17 +986,131 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8785D29-3A1D-EB46-945C-69E7E6633D50}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="8" customFormat="1" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>